<commit_message>
$ Acknowledgement Implemented $
</commit_message>
<xml_diff>
--- a/bootloaderTODO.xlsx
+++ b/bootloaderTODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>CRC32 calculated value in STM and python shall be same</t>
   </si>
@@ -59,6 +59,9 @@
 Send the LED delay from python and verify CRC in STM,
 if CRC matches then modify the delay of LED 
 Data reception in UART interrupt mode</t>
+  </si>
+  <si>
+    <t>Establish Acknowledgement based communicaton</t>
   </si>
 </sst>
 </file>
@@ -115,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -134,6 +137,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E13"/>
+  <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" activeCellId="1" sqref="D15 F11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -460,50 +466,61 @@
       </c>
     </row>
     <row r="3" spans="3:5" ht="57.6">
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="3:5" ht="43.2">
-      <c r="D4" s="4" t="s">
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5">
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="43.2">
+      <c r="D5" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5">
-      <c r="D5" s="5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="3:5">
       <c r="D6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="3:5">
       <c r="D7" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="3:5">
       <c r="D8" s="5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="3:5">
       <c r="D9" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="3:5">
       <c r="D10" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5">
+      <c r="D11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:5">
-      <c r="C13" s="2" t="s">
+    <row r="14" spans="3:5">
+      <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
$ BootLoader Application V1.0 $
Implemented Get Version and Get CID
</commit_message>
<xml_diff>
--- a/bootloaderTODO.xlsx
+++ b/bootloaderTODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>CRC32 calculated value in STM and python shall be same</t>
   </si>
@@ -62,6 +62,45 @@
   </si>
   <si>
     <t>Establish Acknowledgement based communicaton</t>
+  </si>
+  <si>
+    <t>Bootloader commands</t>
+  </si>
+  <si>
+    <t>Erase Application</t>
+  </si>
+  <si>
+    <t>Erases all the Application Memory</t>
+  </si>
+  <si>
+    <t>Check Application Integrity</t>
+  </si>
+  <si>
+    <t>Calculate the CRC of Application and Verify it with CRC already STORED</t>
+  </si>
+  <si>
+    <t>Flash Application</t>
+  </si>
+  <si>
+    <t>Bootloader Version</t>
+  </si>
+  <si>
+    <t>Cchip Identification Number</t>
+  </si>
+  <si>
+    <t>0xB1</t>
+  </si>
+  <si>
+    <t>0xB2</t>
+  </si>
+  <si>
+    <t>0xB3</t>
+  </si>
+  <si>
+    <t>0xB4</t>
+  </si>
+  <si>
+    <t>0xB5</t>
   </si>
 </sst>
 </file>
@@ -130,9 +169,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -141,6 +177,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,21 +472,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E14"/>
+  <dimension ref="B1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="8.88671875" style="2"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="53.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="53.109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="2"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5">
+    <row r="1" spans="3:11">
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
@@ -457,7 +495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="3:5">
+    <row r="2" spans="3:11">
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
@@ -465,62 +503,114 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="3:5" ht="57.6">
-      <c r="D3" s="7" t="s">
+    <row r="3" spans="3:11" ht="57.6">
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="3:5">
-      <c r="D4" s="7" t="s">
+    <row r="4" spans="3:11">
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="3:5" ht="43.2">
-      <c r="D5" s="4" t="s">
+    <row r="5" spans="3:11" ht="43.2">
+      <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="3:5">
-      <c r="D6" s="5" t="s">
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11">
+      <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:5">
-      <c r="D7" s="5" t="s">
+    <row r="7" spans="3:11">
+      <c r="D7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:5">
-      <c r="D8" s="5" t="s">
+    <row r="8" spans="3:11">
+      <c r="D8" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="3:5">
-      <c r="D9" s="5" t="s">
+      <c r="J8" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11">
+      <c r="D9" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="3:5">
-      <c r="D10" s="5" t="s">
+      <c r="H9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11">
+      <c r="D10" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="3:5">
-      <c r="D11" s="5" t="s">
+      <c r="H10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11">
+      <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="3:5">
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11">
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11">
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11">
       <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
$ Erase n Flash Appl Implemented - WORKING $
sample ledBlinking Application bin is added
</commit_message>
<xml_diff>
--- a/bootloaderTODO.xlsx
+++ b/bootloaderTODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
   <si>
     <t>CRC32 calculated value in STM and python shall be same</t>
   </si>
@@ -101,6 +101,44 @@
   </si>
   <si>
     <t>0xB5</t>
+  </si>
+  <si>
+    <t>CMD</t>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
+    <t>ACK</t>
+  </si>
+  <si>
+    <t>LEN.NEXT.PACK</t>
+  </si>
+  <si>
+    <t>PACKET</t>
+  </si>
+  <si>
+    <t>END.PACK</t>
+  </si>
+  <si>
+    <t>LEN.NEXT.PACK - 2BYTES</t>
+  </si>
+  <si>
+    <t>End pack is length of 4 bytes with CRC of complete BIN file, 
+Similaryly STM also calculates the CRC of whole data in PFLASH and sends it to Python.
+Python Compares the CRC with calculated CRC and confirms if Application is flashed successfully.</t>
+  </si>
+  <si>
+    <t>Implement Jump to bootloader command in python</t>
+  </si>
+  <si>
+    <t>NO.OF.PACKTES - 2Bytes</t>
+  </si>
+  <si>
+    <t>0xB6</t>
+  </si>
+  <si>
+    <t>Jump to Application</t>
   </si>
 </sst>
 </file>
@@ -131,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +179,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -157,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,6 +222,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:K14"/>
+  <dimension ref="B1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -484,6 +532,7 @@
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="53.109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="2"/>
+    <col min="8" max="8" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -528,26 +577,38 @@
       </c>
     </row>
     <row r="6" spans="3:11">
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="3:11">
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="3:11">
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="6" t="s">
         <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="3:11">
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="6" t="s">
         <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>9</v>
@@ -560,8 +621,11 @@
       </c>
     </row>
     <row r="10" spans="3:11">
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="6" t="s">
         <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>9</v>
@@ -574,8 +638,14 @@
       </c>
     </row>
     <row r="11" spans="3:11">
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="6" t="s">
         <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="I11" t="s">
         <v>24</v>
@@ -588,14 +658,20 @@
       </c>
     </row>
     <row r="12" spans="3:11">
+      <c r="D12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I12" t="s">
         <v>25</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="3:11">
@@ -603,7 +679,10 @@
         <v>26</v>
       </c>
       <c r="J13" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="K13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="3:11">
@@ -612,6 +691,153 @@
       </c>
       <c r="D14" s="5" t="s">
         <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="7:10">
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="7:10">
+      <c r="G19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="7:10">
+      <c r="G20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="7:10">
+      <c r="G21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="7:10">
+      <c r="G22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="7:10">
+      <c r="G23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="7:10">
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="7:10">
+      <c r="G25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="7:10">
+      <c r="G26" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="7:10">
+      <c r="G27" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="7:10">
+      <c r="G28" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="7:10">
+      <c r="G29" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="7:10" ht="187.2">
+      <c r="H30" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>